<commit_message>
chore: Refactor alumni route to include employment status breakdown by industry and handle errors
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -31,58 +31,49 @@
     <t>company_name</t>
   </si>
   <si>
-    <t>Ram</t>
+    <t>Raman</t>
   </si>
   <si>
     <t>2024-08-04</t>
   </si>
   <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>FinBank</t>
+  </si>
+  <si>
+    <t>Shayam</t>
+  </si>
+  <si>
+    <t>2023-07-14</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>2022-09-30</t>
+  </si>
+  <si>
     <t>UnEmployed</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>BestCorp</t>
-  </si>
-  <si>
-    <t>Shyam</t>
-  </si>
-  <si>
-    <t>2023-07-14</t>
-  </si>
-  <si>
-    <t>Employed</t>
-  </si>
-  <si>
-    <t>Banking</t>
-  </si>
-  <si>
-    <t>FinBank</t>
-  </si>
-  <si>
-    <t>Sahil</t>
-  </si>
-  <si>
-    <t>2022-09-30</t>
-  </si>
-  <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
-    <t>HealthFirst</t>
-  </si>
-  <si>
-    <t>Suraj</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>rasat</t>
   </si>
   <si>
     <t>2021-06-20</t>
   </si>
   <si>
-    <t>TechWave</t>
-  </si>
-  <si>
-    <t>Piyush</t>
+    <t>sdfa</t>
   </si>
   <si>
     <t>2024-01-13</t>
@@ -91,10 +82,7 @@
     <t>Education</t>
   </si>
   <si>
-    <t>EduCare</t>
-  </si>
-  <si>
-    <t>JAW</t>
+    <t>dsfs</t>
   </si>
   <si>
     <t>2023-03-28</t>
@@ -103,49 +91,33 @@
     <t>Finance</t>
   </si>
   <si>
-    <t>CreditWise</t>
-  </si>
-  <si>
-    <t>JOYA</t>
+    <t>NA
+NA
+NA</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
   </si>
   <si>
     <t>2022-11-05</t>
   </si>
   <si>
-    <t>WebMinds</t>
-  </si>
-  <si>
-    <t>SWETA Gupta</t>
+    <t>fsfd</t>
   </si>
   <si>
     <t>2023-02-17</t>
   </si>
   <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>MarketPlus</t>
-  </si>
-  <si>
-    <t>ArjWN</t>
-  </si>
-  <si>
     <t>2021-08-10</t>
   </si>
   <si>
-    <t>SafeBank</t>
-  </si>
-  <si>
-    <t>Rani Desai</t>
+    <t>ShopEase</t>
+  </si>
+  <si>
+    <t>sdfsdf</t>
   </si>
   <si>
     <t>2022-12-22</t>
-  </si>
-  <si>
-    <t>Retail</t>
-  </si>
-  <si>
-    <t>ShopEase</t>
   </si>
 </sst>
 </file>
@@ -163,7 +135,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -195,16 +167,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,18 +492,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -538,11 +516,11 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -555,157 +533,157 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>